<commit_message>
Updated TMS_PCMs.xlsx from OneDrive
</commit_message>
<xml_diff>
--- a/TMS_PCMs.xlsx
+++ b/TMS_PCMs.xlsx
@@ -306,7 +306,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TT-20251024000043</t>
+          <t>TT-20251024000052</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -326,7 +326,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-10-24 03:23:39</t>
+          <t>2025-10-24 04:26:39</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -341,22 +341,22 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>HAW0293</t>
+          <t>MKTF0647</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Region_4</t>
+          <t>Region_5</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Sceco</t>
+          <t>Generator_SG</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000171</t>
+          <t>PCM-20251024-00000228</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -371,12 +371,12 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>1(2G/3G/5G) sites down under HAW0293-P2/HAW0293-P2 @ Sceco</t>
+          <t>1(2G/3G) sites down under MKTF0647-P1-USF/MKTF0647-P1-USF @ Generator_SG</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -391,12 +391,12 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000171</t>
+          <t>PCM-20251024-00000228</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>TT-20251024-00200</t>
+          <t>TT-20251024-00268</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -411,12 +411,12 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Major</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>2025-10-24 03:15:23</t>
+          <t>2025-10-24 04:18:33</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -441,7 +441,7 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>2025-10-24 03:15:23</t>
+          <t>2025-10-24 04:18:33</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
@@ -471,7 +471,7 @@
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000171</t>
+          <t>PCM-20251024-00000228</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>HAW0293</t>
+          <t>MKTF0647</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>taif</t>
+          <t>makkah</t>
         </is>
       </c>
       <c r="AN2" t="inlineStr">
@@ -521,17 +521,17 @@
       </c>
       <c r="AS2" t="inlineStr">
         <is>
-          <t>HAW0293-P2</t>
+          <t>MKTF0647-P1-USF</t>
         </is>
       </c>
       <c r="AT2" t="inlineStr">
         <is>
-          <t>SERIAL-20251024-0042</t>
+          <t>SERIAL-20251024-0052</t>
         </is>
       </c>
       <c r="AU2" t="inlineStr">
         <is>
-          <t>2025-10-24 03:15:26</t>
+          <t>2025-10-24 04:18:36</t>
         </is>
       </c>
     </row>
@@ -543,7 +543,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TT-20251024000039</t>
+          <t>TT-20251024000050</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-10-24 03:14:39</t>
+          <t>2025-10-24 04:17:24</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -578,22 +578,22 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>MAK2246</t>
+          <t>HMBY2212</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Region_5</t>
+          <t>Region_1</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Sceco</t>
+          <t>Generator_SG</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000161</t>
+          <t>PCM-20251024-00000218</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>1(2G/LTE/5G) sites down under MAK2246-P3/MAK2246-P3 @ Sceco</t>
+          <t>2(2G) 1(3G) 2(LTE) sites down under HMBY2212-P3,KBR2492-P3/DM1MBSCH01 @ Sceco</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -628,12 +628,12 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000161</t>
+          <t>PCM-20251024-00000218</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>TT-20251024-00182</t>
+          <t>TT-20251024-00248</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>BTS O&amp;M LINK FAILURE</t>
+          <t>CSL Fault</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
@@ -653,22 +653,22 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>2025-10-24 03:06:22</t>
+          <t>2025-10-24 04:07:15</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>2G_LTE_5G SA</t>
+          <t>2G_3G_LTE SA</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>7706</t>
+          <t>21825</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>BTS O&amp;M LINK FAILURE</t>
+          <t>CSL Fault</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>2025-10-24 03:06:22</t>
+          <t>2025-10-24 04:07:15</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
@@ -688,17 +688,23 @@
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t/>
+          <t>Dear Team,
+Hub:- HMBY2212
+Suspecting power issue at hub site and kindly send EM-FLM team to check and resolve issue at site.
+Kindly update TT under EM FLM</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t/>
+          <t>Dear Team,
+Hub:- HMBY2212
+Suspecting power issue at hub site and kindly send EM-FLM team to check and resolve issue at site.
+Kindly update TT under EM FLM</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t/>
+          <t>PCM-20251024-00000215</t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
@@ -708,7 +714,7 @@
       </c>
       <c r="AI3" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000161</t>
+          <t>PCM-20251024-00000218</t>
         </is>
       </c>
       <c r="AJ3" t="inlineStr">
@@ -718,7 +724,7 @@
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>MAK2246</t>
+          <t>HMBY2212</t>
         </is>
       </c>
       <c r="AL3" t="inlineStr">
@@ -728,7 +734,7 @@
       </c>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>makkah</t>
+          <t>dammam</t>
         </is>
       </c>
       <c r="AN3" t="inlineStr">
@@ -738,12 +744,12 @@
       </c>
       <c r="AO3" t="inlineStr">
         <is>
-          <t>EM</t>
+          <t>Telecom</t>
         </is>
       </c>
       <c r="AP3" t="inlineStr">
         <is>
-          <t>2G</t>
+          <t>SRAN</t>
         </is>
       </c>
       <c r="AQ3" t="inlineStr">
@@ -758,17 +764,17 @@
       </c>
       <c r="AS3" t="inlineStr">
         <is>
-          <t>MAK2246-P3</t>
+          <t>KBR2492-P3 2G_LTE,HMBY2212-P3 2G_3G_LTE</t>
         </is>
       </c>
       <c r="AT3" t="inlineStr">
         <is>
-          <t>SERIAL-20251024-0039</t>
+          <t>SERIAL-20251024-0050</t>
         </is>
       </c>
       <c r="AU3" t="inlineStr">
         <is>
-          <t>2025-10-24 03:06:26</t>
+          <t>2025-10-24 04:07:17</t>
         </is>
       </c>
     </row>
@@ -780,7 +786,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TT-20251024000028</t>
+          <t>TT-20251024000043</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -800,7 +806,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-10-24 02:23:59</t>
+          <t>2025-10-24 03:23:39</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -815,12 +821,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>MAK0195</t>
+          <t>HAW0293</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Region_5</t>
+          <t>Region_4</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -830,7 +836,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000121</t>
+          <t>PCM-20251024-00000171</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -845,12 +851,12 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>1(2G/5G) sites down under MAK0195-P1-HUB/MAK0195-P1-HUB @ Sceco</t>
+          <t>1(2G/3G/5G) sites down under HAW0293-P2/HAW0293-P2 @ Sceco</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -865,12 +871,12 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000121</t>
+          <t>PCM-20251024-00000171</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>TT-20251024-00113</t>
+          <t>TT-20251024-00200</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -885,17 +891,17 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Major</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>2025-10-24 01:51:15</t>
+          <t>2025-10-24 03:15:23</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>2G SA</t>
+          <t>2G_3G SA</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
@@ -915,7 +921,7 @@
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>2025-10-24 01:51:15</t>
+          <t>2025-10-24 03:15:23</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
@@ -925,17 +931,17 @@
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>Power issue at site</t>
+          <t/>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>Power issue at site</t>
+          <t/>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000102</t>
+          <t/>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
@@ -945,7 +951,7 @@
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000121</t>
+          <t>PCM-20251024-00000171</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
@@ -955,7 +961,7 @@
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>MAK0195</t>
+          <t>HAW0293</t>
         </is>
       </c>
       <c r="AL4" t="inlineStr">
@@ -965,7 +971,7 @@
       </c>
       <c r="AM4" t="inlineStr">
         <is>
-          <t>makkah</t>
+          <t>taif</t>
         </is>
       </c>
       <c r="AN4" t="inlineStr">
@@ -995,17 +1001,17 @@
       </c>
       <c r="AS4" t="inlineStr">
         <is>
-          <t>MAK0195-P1-HUB</t>
+          <t>HAW0293-P2</t>
         </is>
       </c>
       <c r="AT4" t="inlineStr">
         <is>
-          <t>SERIAL-20251024-0028</t>
+          <t>SERIAL-20251024-0042</t>
         </is>
       </c>
       <c r="AU4" t="inlineStr">
         <is>
-          <t>2025-10-24 01:51:23</t>
+          <t>2025-10-24 03:15:26</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1023,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TT-20251024000023</t>
+          <t>TT-20251024000028</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1037,7 +1043,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-10-24 02:09:09</t>
+          <t>2025-10-24 02:23:59</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1052,22 +1058,22 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>HMBY0419</t>
+          <t>MAK0195</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Region_1</t>
+          <t>Region_5</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Generator_SG</t>
+          <t>Sceco</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000107</t>
+          <t>PCM-20251024-00000121</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -1082,12 +1088,12 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>1(2G/LTE) sites down under HMBY0419-P3/DM1MBSCH01 @ Generator_SG</t>
+          <t>1(2G/5G) sites down under MAK0195-P1-HUB/MAK0195-P1-HUB @ Sceco</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>P3</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -1102,12 +1108,12 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000107</t>
+          <t>PCM-20251024-00000121</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>TT-20251024-00121</t>
+          <t>TT-20251024-00113</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -1117,32 +1123,32 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>CSL Fault</t>
+          <t>BTS O&amp;M LINK FAILURE</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>Major</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>2025-10-24 02:00:47</t>
+          <t>2025-10-24 01:51:15</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>2G_LTE SA</t>
+          <t>2G SA</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>21825</t>
+          <t>7706</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>CSL Fault</t>
+          <t>BTS O&amp;M LINK FAILURE</t>
         </is>
       </c>
       <c r="AB5" t="inlineStr">
@@ -1152,7 +1158,7 @@
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>2025-10-24 02:00:47</t>
+          <t>2025-10-24 01:51:15</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
@@ -1162,17 +1168,17 @@
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t/>
+          <t>Power issue at site</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t/>
+          <t>Power issue at site</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t/>
+          <t>PCM-20251024-00000102</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
@@ -1182,7 +1188,7 @@
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000107</t>
+          <t>PCM-20251024-00000121</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
@@ -1192,7 +1198,7 @@
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>HMBY0419</t>
+          <t>MAK0195</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr">
@@ -1202,7 +1208,7 @@
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>dammam</t>
+          <t>makkah</t>
         </is>
       </c>
       <c r="AN5" t="inlineStr">
@@ -1232,17 +1238,17 @@
       </c>
       <c r="AS5" t="inlineStr">
         <is>
-          <t>HMBY0419-P3</t>
+          <t>MAK0195-P1-HUB</t>
         </is>
       </c>
       <c r="AT5" t="inlineStr">
         <is>
-          <t>SERIAL-20251024-0023</t>
+          <t>SERIAL-20251024-0028</t>
         </is>
       </c>
       <c r="AU5" t="inlineStr">
         <is>
-          <t>2025-10-24 02:00:49</t>
+          <t>2025-10-24 01:51:23</t>
         </is>
       </c>
     </row>
@@ -1254,7 +1260,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TT-20251024000009</t>
+          <t>TT-20251024000023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1274,7 +1280,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-10-24 01:01:29</t>
+          <t>2025-10-24 02:09:09</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1289,22 +1295,22 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>RIY0854</t>
+          <t>HMBY0419</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Region_2</t>
+          <t>Region_1</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Sceco</t>
+          <t>Generator_SG</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000051</t>
+          <t>PCM-20251024-00000107</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -1319,12 +1325,12 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>3(2G) 3(LTE) sites down under RIYA6185-P2,RIY0854-P1-VIP,RIY0405-P2/R2_RY1_HWBSC01 @ Sceco</t>
+          <t>1(2G/LTE) sites down under HMBY0419-P3/DM1MBSCH01 @ Generator_SG</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>VIP</t>
+          <t>P3</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -1339,12 +1345,12 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000051</t>
+          <t>PCM-20251024-00000107</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>TT-20251024-00049</t>
+          <t>TT-20251024-00121</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -1359,12 +1365,12 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Major</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>2025-10-24 00:51:40</t>
+          <t>2025-10-24 02:00:47</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -1389,7 +1395,7 @@
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>2025-10-24 00:51:40</t>
+          <t>2025-10-24 02:00:47</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
@@ -1399,23 +1405,17 @@
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>Dear Team,
-Hub:- RIY0854
-Suspecting power issue at hub site and kindly send EM-FLM team to check and resolve issue at site.
-Kindly update TT under EM FLM</t>
+          <t/>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>Dear Team,
-Hub:- RIY0854
-Suspecting power issue at hub site and kindly send EM-FLM team to check and resolve issue at site.
-Kindly update TT under EM FLM</t>
+          <t/>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000048</t>
+          <t/>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>PCM-20251024-00000051</t>
+          <t>PCM-20251024-00000107</t>
         </is>
       </c>
       <c r="AJ6" t="inlineStr">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>RIY0854</t>
+          <t>HMBY0419</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>riyadh</t>
+          <t>dammam</t>
         </is>
       </c>
       <c r="AN6" t="inlineStr">
@@ -1455,12 +1455,12 @@
       </c>
       <c r="AO6" t="inlineStr">
         <is>
-          <t>Telecom</t>
+          <t>EM</t>
         </is>
       </c>
       <c r="AP6" t="inlineStr">
         <is>
-          <t>SRAN</t>
+          <t>2G</t>
         </is>
       </c>
       <c r="AQ6" t="inlineStr">
@@ -1475,17 +1475,17 @@
       </c>
       <c r="AS6" t="inlineStr">
         <is>
-          <t>RIYA6185-P2 2G_LTE,RIY0854-P1-VIP 2G_LTE,RIY0405-P2 2G_LTE</t>
+          <t>HMBY0419-P3</t>
         </is>
       </c>
       <c r="AT6" t="inlineStr">
         <is>
-          <t>SERIAL-20251024-0009</t>
+          <t>SERIAL-20251024-0023</t>
         </is>
       </c>
       <c r="AU6" t="inlineStr">
         <is>
-          <t>2025-10-24 00:51:45</t>
+          <t>2025-10-24 02:00:49</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Warning</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">

</xml_diff>